<commit_message>
built helper functions for date, plural
</commit_message>
<xml_diff>
--- a/documents/table_relationships.xlsx
+++ b/documents/table_relationships.xlsx
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +92,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -301,8 +303,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1619640" y="415440"/>
-          <a:ext cx="954360" cy="463680"/>
+          <a:off x="1621080" y="415440"/>
+          <a:ext cx="955440" cy="463680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -342,8 +344,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2580120" y="1300320"/>
-          <a:ext cx="1214280" cy="735120"/>
+          <a:off x="2582640" y="1300320"/>
+          <a:ext cx="1216440" cy="735120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -383,7 +385,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3394080" y="391320"/>
+          <a:off x="3398760" y="391320"/>
           <a:ext cx="412560" cy="903240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -466,7 +468,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="418680" y="1173960"/>
-          <a:ext cx="1188720" cy="692280"/>
+          <a:ext cx="1190160" cy="692280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -497,10 +499,10 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.55"/>
   </cols>

</xml_diff>